<commit_message>
Fixed mistakes in precedence table
</commit_message>
<xml_diff>
--- a/grammar/precedence_table.xlsx
+++ b/grammar/precedence_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vojon\Documents\Škola\3_sem\IFJ\projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F365083-6255-47C8-93FD-D01B49C2032F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5468130-9F73-4E18-8200-4B41135255D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BDF90FF-C416-42E4-952D-EAE081E666E6}"/>
+    <workbookView xWindow="13845" yWindow="1530" windowWidth="14220" windowHeight="11370" xr2:uid="{4BDF90FF-C416-42E4-952D-EAE081E666E6}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1371,8 +1371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F1133E-67C6-40F5-ACA7-E7093B96C824}">
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W17" sqref="W17"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,10 +1443,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>9</v>
@@ -1505,7 +1505,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="53" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="54" t="s">
         <v>9</v>
@@ -1871,10 +1871,10 @@
         <v>7</v>
       </c>
       <c r="G9" s="23" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I9" s="25" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Fixed asociativity of .. (look at preceence table)
</commit_message>
<xml_diff>
--- a/grammar/precedence_table.xlsx
+++ b/grammar/precedence_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vojon\Documents\Škola\3_sem\IFJ\projekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5468130-9F73-4E18-8200-4B41135255D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A20C673-4A55-4628-9906-7B92FB73F3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13845" yWindow="1530" windowWidth="14220" windowHeight="11370" xr2:uid="{4BDF90FF-C416-42E4-952D-EAE081E666E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4BDF90FF-C416-42E4-952D-EAE081E666E6}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -1059,7 +1059,18 @@
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1372,7 +1383,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1888,7 @@
         <v>7</v>
       </c>
       <c r="I9" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J9" s="29" t="s">
         <v>9</v>
@@ -2487,6 +2498,11 @@
       <c r="S19" s="49"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:S19">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"&lt;"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>